<commit_message>
cleaned out screenshot as file code, updated test codes, added more driver methods
</commit_message>
<xml_diff>
--- a/src/test/java/com/github/GandhiTC/java/ThreadsafeFrameWork/testData/LoginData.xlsx
+++ b/src/test/java/com/github/GandhiTC/java/ThreadsafeFrameWork/testData/LoginData.xlsx
@@ -51,10 +51,10 @@
     <t>nesAjap</t>
   </si>
   <si>
-    <t>mngr247214</t>
-  </si>
-  <si>
-    <t>AzEgEnu</t>
+    <t>mngr250218</t>
+  </si>
+  <si>
+    <t>vezYgad</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated test site credentials
</commit_message>
<xml_diff>
--- a/src/test/java/com/github/GandhiTC/java/ThreadsafeFrameWork/testData/LoginData.xlsx
+++ b/src/test/java/com/github/GandhiTC/java/ThreadsafeFrameWork/testData/LoginData.xlsx
@@ -21,12 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>mngr83460</t>
-  </si>
-  <si>
-    <t>qAbUzyj</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -37,6 +31,12 @@
   </si>
   <si>
     <t>vezYgad</t>
+  </si>
+  <si>
+    <t>mngr266814</t>
+  </si>
+  <si>
+    <t>vAtarEt</t>
   </si>
 </sst>
 </file>
@@ -438,26 +438,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>